<commit_message>
drill down system tab clockin
</commit_message>
<xml_diff>
--- a/data/AutomationChips.xlsx
+++ b/data/AutomationChips.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesystems_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesystems-my.sharepoint.com/personal/prasad_kamble_wdtablesystems_com/Documents/Documents/PlayWrightProject/PlayWright_POC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19087DDE-7D4D-4CC8-B51B-5D3F5B6DB657}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CF2223F-E204-4DB1-96F5-E61E41FABAE1}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ChipIds" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
   <si>
     <t>T</t>
   </si>
@@ -558,7 +558,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +903,9 @@
       <c r="B31" s="1">
         <v>500</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -912,7 +914,9 @@
       <c r="B32" s="1">
         <v>500</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -921,7 +925,9 @@
       <c r="B33" s="1">
         <v>500</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -930,7 +936,9 @@
       <c r="B34" s="1">
         <v>500</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -939,7 +947,9 @@
       <c r="B35" s="1">
         <v>500</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -948,7 +958,9 @@
       <c r="B36" s="1">
         <v>500</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -957,7 +969,9 @@
       <c r="B37" s="1">
         <v>500</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -966,7 +980,9 @@
       <c r="B38" s="1">
         <v>500</v>
       </c>
-      <c r="C38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -975,7 +991,9 @@
       <c r="B39" s="1">
         <v>500</v>
       </c>
-      <c r="C39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -984,7 +1002,9 @@
       <c r="B40" s="1">
         <v>500</v>
       </c>
-      <c r="C40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">

</xml_diff>